<commit_message>
Final cleanup - BOM
</commit_message>
<xml_diff>
--- a/- PCB -/Full BOM.xlsx
+++ b/- PCB -/Full BOM.xlsx
@@ -1,6 +1,6 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" mc:Ignorable="x15 xr xr6 xr10">
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26501"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\MenMe\Рабочий стол\GitHub\RoboCop\- PCB -\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{8731463C-D5DB-4F5D-92A8-508993F5D3E0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6CABDBD6-0401-4276-B404-4E3B22170DC3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="SUMEC FULL BOM" sheetId="1" r:id="rId1"/>
@@ -196,8 +196,8 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <fonts count="19" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <fonts count="20" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -334,6 +334,12 @@
     </font>
     <font>
       <sz val="11"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="8"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -1111,11 +1117,11 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="B2:F26"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="95" zoomScaleNormal="95" workbookViewId="0">
-      <selection activeCell="J16" sqref="J16"/>
+    <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="J17" sqref="J17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -1501,6 +1507,8 @@
       </c>
     </row>
   </sheetData>
+  <phoneticPr fontId="19" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>